<commit_message>
Actualización plantilla de casos de uso
</commit_message>
<xml_diff>
--- a/Documents/Plantilla_Lista_de_Tareas_de_la_Iteración.xlsx
+++ b/Documents/Plantilla_Lista_de_Tareas_de_la_Iteración.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vik-t\Documents\SoftwareEngineering\6toSemestre\DesarrolloDeSoftware\PANGEA\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE297BA9-133A-436C-BA65-4DBAC1C2C7A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -15,8 +21,16 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -168,7 +182,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -650,75 +664,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BA17"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.6640625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="2.6640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="2.6640625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="2.6640625" style="2" customWidth="1"/>
-    <col min="23" max="23" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="2.6640625" style="2" customWidth="1"/>
-    <col min="26" max="26" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="2.6640625" style="2" customWidth="1"/>
-    <col min="29" max="29" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="2.6640625" style="2" customWidth="1"/>
-    <col min="32" max="32" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="2.6640625" style="2" customWidth="1"/>
-    <col min="35" max="35" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="2.6640625" style="2" customWidth="1"/>
-    <col min="38" max="38" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="2.6640625" style="2" customWidth="1"/>
-    <col min="41" max="41" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="2.6640625" style="2" customWidth="1"/>
-    <col min="44" max="44" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="2.6640625" style="2" customWidth="1"/>
-    <col min="47" max="47" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="2.6640625" style="2" customWidth="1"/>
-    <col min="50" max="50" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="5.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="1.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="2.7109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="2.7109375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="2.7109375" style="2" customWidth="1"/>
+    <col min="29" max="29" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="2.7109375" style="2" customWidth="1"/>
+    <col min="32" max="32" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="2.7109375" style="2" customWidth="1"/>
+    <col min="35" max="35" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="2.7109375" style="2" customWidth="1"/>
+    <col min="38" max="38" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="2.7109375" style="2" customWidth="1"/>
+    <col min="41" max="41" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="2.7109375" style="2" customWidth="1"/>
+    <col min="44" max="44" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="2.7109375" style="2" customWidth="1"/>
+    <col min="47" max="47" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="2.7109375" style="2" customWidth="1"/>
+    <col min="50" max="50" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="5.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:53" ht="28">
+    <row r="1" spans="2:53" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="12" t="s">
         <v>44</v>
       </c>
@@ -726,15 +740,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="2:53" ht="28">
+    <row r="2" spans="2:53" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="12"/>
     </row>
-    <row r="3" spans="2:53" ht="20">
+    <row r="3" spans="2:53" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:53" ht="14" customHeight="1">
+    <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H4" s="14" t="s">
         <v>9</v>
       </c>
@@ -814,7 +828,7 @@
       </c>
       <c r="BA4" s="15"/>
     </row>
-    <row r="5" spans="2:53" ht="28">
+    <row r="5" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>32</v>
       </c>
@@ -944,7 +958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:53">
+    <row r="6" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
         <v>31</v>
       </c>
@@ -1053,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:53">
+    <row r="7" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
@@ -1160,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:53">
+    <row r="8" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
@@ -1267,7 +1281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:53">
+    <row r="9" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
@@ -1374,7 +1388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:53">
+    <row r="10" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
         <v>31</v>
       </c>
@@ -1483,7 +1497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:53">
+    <row r="11" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
@@ -1590,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:53">
+    <row r="12" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
@@ -1697,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:53">
+    <row r="13" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
@@ -1804,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:53">
+    <row r="14" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
         <v>31</v>
       </c>
@@ -1913,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:53">
+    <row r="15" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5" t="s">
@@ -2020,7 +2034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:53">
+    <row r="16" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
@@ -2127,7 +2141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:53">
+    <row r="17" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
@@ -2236,6 +2250,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2247,13 +2266,9 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <colBreaks count="3" manualBreakCount="3">
     <brk id="21" max="18" man="1"/>
     <brk id="36" max="18" man="1"/>
@@ -2268,33 +2283,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="1.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="86" style="4" customWidth="1"/>
-    <col min="4" max="4" width="2.83203125" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="4"/>
+    <col min="4" max="4" width="2.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="10.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="28">
+    <row r="1" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="20">
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2302,7 +2317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="28">
+    <row r="5" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="str">
         <f>'Casos de Uso'!B5</f>
         <v>Identificador (ID) de CU</v>
@@ -2311,7 +2326,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="28">
+    <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="str">
         <f>'Casos de Uso'!C5</f>
         <v>Elemento</v>
@@ -2320,7 +2335,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="42">
+    <row r="7" spans="2:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
@@ -2328,7 +2343,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="42">
+    <row r="8" spans="2:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>42</v>
       </c>
@@ -2336,7 +2351,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="28">
+    <row r="9" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
@@ -2344,7 +2359,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="28">
+    <row r="10" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
@@ -2352,7 +2367,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="28">
+    <row r="11" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>27</v>
       </c>
@@ -2360,7 +2375,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
@@ -2368,7 +2383,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="42">
+    <row r="13" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
@@ -2376,7 +2391,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="28">
+    <row r="14" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>26</v>
       </c>
@@ -2386,6 +2401,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>